<commit_message>
Completed geneRNASeq stress, and its PCA stress
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/pca/stress_results.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/other_dr_techniques/pca/stress_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -966,6 +966,98 @@
         <v>6.63205079892673e-05</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-08-26 00:57:59</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>geneRNASeq</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>30</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.1504038410748585</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-08-26 00:57:59</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>geneRNASeq</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>40</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.1373159283965877</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-08-26 00:57:59</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>geneRNASeq</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.2094341651276703</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2023-08-26 00:57:59</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>geneRNASeq</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>def</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>20</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.170001274791034</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>